<commit_message>
Add WARP1_TEST1 sample plate with 6144 fake samples.
</commit_message>
<xml_diff>
--- a/app/seed_data/smt_seed_data.xlsx
+++ b/app/seed_data/smt_seed_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="-23120" windowWidth="25600" windowHeight="15520" tabRatio="801" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="801" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sample_transfer_type" sheetId="35" r:id="rId1"/>
@@ -4217,12 +4217,13 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5416,8 +5417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5655,7 +5656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>26</v>
       </c>
@@ -5666,7 +5667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>27</v>
       </c>
@@ -5677,7 +5678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>28</v>
       </c>
@@ -5688,7 +5689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>29</v>
       </c>
@@ -5699,7 +5700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>30</v>
       </c>
@@ -5710,7 +5711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>31</v>
       </c>
@@ -5721,7 +5722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>32</v>
       </c>
@@ -5732,7 +5733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>33</v>
       </c>
@@ -5743,7 +5744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>34</v>
       </c>
@@ -5753,8 +5754,14 @@
       <c r="C25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25">
+        <v>6144</v>
+      </c>
+      <c r="E25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>35</v>
       </c>
@@ -5765,7 +5772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>36</v>
       </c>
@@ -5776,7 +5783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>37</v>
       </c>
@@ -14430,7 +14437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix for 48-well plates.
</commit_message>
<xml_diff>
--- a/app/seed_data/smt_seed_data.xlsx
+++ b/app/seed_data/smt_seed_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="801" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="801" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sample_transfer_type" sheetId="35" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="1151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="1152">
   <si>
     <t>description</t>
   </si>
@@ -3476,6 +3476,9 @@
   </si>
   <si>
     <t>destination_plate_size</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
   </si>
 </sst>
 </file>
@@ -4217,7 +4220,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5417,8 +5420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5809,8 +5812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5929,6 +5932,12 @@
       </c>
       <c r="F5" t="s">
         <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8">

</xml_diff>